<commit_message>
Added VGG16 for augmentation
</commit_message>
<xml_diff>
--- a/Experiment checklist.xlsx
+++ b/Experiment checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE11FAF-90FD-48B2-8FC3-C190599BF96F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CDB800-9635-49B8-BC62-10A11A1B301D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,22 +465,22 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.68359375" customWidth="1"/>
-    <col min="2" max="2" width="19.578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.62890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.3671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -496,7 +496,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="3" t="s">
@@ -518,7 +518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -532,7 +532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -558,7 +558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -572,7 +572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -586,7 +586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -600,7 +600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -614,7 +614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -640,7 +640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -654,7 +654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Performed Experiment on data7
</commit_message>
<xml_diff>
--- a/Experiment checklist.xlsx
+++ b/Experiment checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D675F6-5695-4DF7-A5B9-54E431307185}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215DC7FB-9F84-475A-9FF1-A0B4292DA92C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Data</t>
   </si>
@@ -471,7 +471,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,12 +710,24 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.93111638954869302</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2">
+        <v>64</v>
+      </c>
       <c r="H10" s="1">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Exp: data8 complete. All data files done.
</commit_message>
<xml_diff>
--- a/Experiment checklist.xlsx
+++ b/Experiment checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215DC7FB-9F84-475A-9FF1-A0B4292DA92C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763C48DA-B4C0-4662-83A9-E3515AE8C9EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Data</t>
   </si>
@@ -471,7 +471,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,11 +737,21 @@
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="C11" s="2">
+        <v>0.93879651623119498</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="2">
+        <v>128</v>
+      </c>
       <c r="H11" s="1">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
data set 0 and 2 done
</commit_message>
<xml_diff>
--- a/Experiment checklist.xlsx
+++ b/Experiment checklist.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763C48DA-B4C0-4662-83A9-E3515AE8C9EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42E8C33-F224-4F0A-824B-6CA3C64F4E8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Step 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="23">
   <si>
     <t>Data</t>
   </si>
@@ -95,10 +96,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -179,6 +187,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -188,6 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,24 +499,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
@@ -736,7 +748,9 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C11" s="2">
         <v>0.93879651623119498</v>
       </c>
@@ -755,6 +769,253 @@
       <c r="H11" s="1">
         <v>15</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DE220F-4E96-4F16-9344-F206B021B01F}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="9">
+        <v>0.94695170230000003</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2">
+        <v>128</v>
+      </c>
+      <c r="H3" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2">
+        <v>128</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2">
+        <v>128</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2">
+        <v>128</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2">
+        <v>64</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2">
+        <v>64</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2">
+        <v>128</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2">
+        <v>64</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="2">
+        <v>128</v>
+      </c>
+      <c r="H11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
set 3 w/o ES
</commit_message>
<xml_diff>
--- a/Experiment checklist.xlsx
+++ b/Experiment checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42E8C33-F224-4F0A-824B-6CA3C64F4E8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB540513-2E38-4CAD-890B-916AF8890019}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
   <si>
     <t>Data</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>0.9469517023 (need to redo - without early stopping)</t>
+  </si>
+  <si>
+    <t>need to redo - without early stopping</t>
   </si>
 </sst>
 </file>
@@ -190,6 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -199,7 +206,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,24 +505,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
@@ -784,36 +790,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DE220F-4E96-4F16-9344-F206B021B01F}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
@@ -838,8 +844,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="9">
-        <v>0.94695170230000003</v>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>21</v>
@@ -882,7 +888,9 @@
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
@@ -902,7 +910,9 @@
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2">
+        <v>0.90981789390340395</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
@@ -915,7 +925,9 @@
       <c r="G6" s="2">
         <v>128</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">

</xml_diff>

<commit_message>
commited step3 without model pkl files
</commit_message>
<xml_diff>
--- a/Experiment checklist.xlsx
+++ b/Experiment checklist.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8454FBCE-8948-40A4-8C95-AFCA9400446A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D3FA40-EDAE-4151-AF76-EF6A2571E85E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1" sheetId="1" r:id="rId1"/>
     <sheet name="Setp 2" sheetId="3" r:id="rId2"/>
     <sheet name="Step 1 vs Step 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Step 3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="33">
   <si>
     <t>Data</t>
   </si>
@@ -97,6 +98,30 @@
   </si>
   <si>
     <t>Step</t>
+  </si>
+  <si>
+    <t>Step 1 Test Acc</t>
+  </si>
+  <si>
+    <t>Step 2 Test Acc</t>
+  </si>
+  <si>
+    <t>Step2  - Step1</t>
+  </si>
+  <si>
+    <t>Improved?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Use Step (1 or 2)</t>
+  </si>
+  <si>
+    <t>Best Step among (1 or 2) and 3</t>
+  </si>
+  <si>
+    <t>Step 1 was better for all data sets</t>
   </si>
 </sst>
 </file>
@@ -180,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -201,6 +226,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -210,9 +241,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,24 +544,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
@@ -810,24 +842,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1091,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B616E44B-A5E7-4616-ABF4-8EC2B6E1EDE4}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,6 +1136,8 @@
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1112,31 +1146,31 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="8" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="J4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1155,7 +1189,7 @@
       <c r="H5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="9"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1200,7 +1234,7 @@
       <c r="J6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="9">
         <v>0.94228028503562899</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -1571,21 +1605,40 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
+    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F18" s="9"/>
+      <c r="K17" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="11"/>
       <c r="G18" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="K18" s="2">
+        <v>0.94742676167854301</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0.94228028503562899</v>
+      </c>
+      <c r="M18">
+        <f>L18-K18</f>
+        <v>-5.1464766429140107E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F19" s="2" t="s">
         <v>2</v>
       </c>
@@ -1595,8 +1648,18 @@
       <c r="H19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="K19" s="2">
+        <v>0.90546318289786198</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.88566904196357799</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ref="M19:M26" si="0">L19-K19</f>
+        <v>-1.9794140934283999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1606,8 +1669,18 @@
       <c r="H20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="K20" s="2">
+        <v>0.90783847980997601</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.88313539192399004</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>-2.4703087885985964E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1617,8 +1690,18 @@
       <c r="H21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="K21" s="2">
+        <v>0.914014251781472</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.905542359461599</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>-8.4718923198729978E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1628,8 +1711,18 @@
       <c r="H22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="K22" s="2">
+        <v>0.940617577197149</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.92098178939034003</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>-1.9635787806808969E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1637,10 +1730,20 @@
         <v>0.940617577197149</v>
       </c>
       <c r="H23" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.94663499604117096</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.93357086302454395</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>-1.3064133016627011E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F24" s="2" t="s">
         <v>6</v>
       </c>
@@ -1648,10 +1751,20 @@
         <v>0.94663499604117096</v>
       </c>
       <c r="H24" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="6:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.93379999999999996</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.90720506730007899</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>-2.659493269992097E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F25" s="2" t="s">
         <v>7</v>
       </c>
@@ -1659,10 +1772,20 @@
         <v>0.93379999999999996</v>
       </c>
       <c r="H25" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="6:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.93111638954869302</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.90332541567695901</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>-2.7790973871734015E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1670,10 +1793,20 @@
         <v>0.93111638954869302</v>
       </c>
       <c r="H26" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="6:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0.93879651623119498</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.92304038004750599</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>-1.5756136183688985E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F27" s="2" t="s">
         <v>9</v>
       </c>
@@ -1681,7 +1814,12 @@
         <v>0.93879651623119498</v>
       </c>
       <c r="H27" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1834,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{BFE24FF7-7917-4E5E-AAD4-ADEEA6AAD807}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{5061348E-7F02-4662-9A06-A4A1FDDB0217}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1707,8 +1845,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Step 1 vs Step 2'!H18:H18</xm:f>
-              <xm:sqref>H18</xm:sqref>
+              <xm:f>'Step 1 vs Step 2'!K5:K5</xm:f>
+              <xm:sqref>K5</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1728,7 +1866,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{5061348E-7F02-4662-9A06-A4A1FDDB0217}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{BFE24FF7-7917-4E5E-AAD4-ADEEA6AAD807}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1739,8 +1877,196 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Step 1 vs Step 2'!K5:K5</xm:f>
-              <xm:sqref>K5</xm:sqref>
+              <xm:f>'Step 1 vs Step 2'!H18:H18</xm:f>
+              <xm:sqref>H18</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E59D2C-663A-42CA-9913-AA1980550302}">
+  <dimension ref="B4:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="11"/>
+      <c r="C5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{9DAB5BC3-0E2E-447E-8E88-AF6AF6B0F3BA}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Step 3'!C5:C5</xm:f>
+              <xm:sqref>C5</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
added data 0 and data 1
</commit_message>
<xml_diff>
--- a/Experiment checklist.xlsx
+++ b/Experiment checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D3FA40-EDAE-4151-AF76-EF6A2571E85E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED280553-7D8D-4D5B-B899-4F3A445D65C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Step 1" sheetId="1" r:id="rId1"/>
     <sheet name="Setp 2" sheetId="3" r:id="rId2"/>
     <sheet name="Step 1 vs Step 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Step 3" sheetId="5" r:id="rId4"/>
+    <sheet name="Step 4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="33">
   <si>
     <t>Data</t>
   </si>
@@ -232,6 +232,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -241,10 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +528,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,24 +544,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
@@ -830,7 +830,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H11"/>
+      <selection activeCell="H11" sqref="A3:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,24 +842,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1091,7 +1091,9 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C11" s="2">
         <v>0.92304038004750599</v>
       </c>
@@ -1118,6 +1120,7 @@
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1126,7 +1129,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="F17" sqref="F17:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,31 +1149,31 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="J4" s="10" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="J4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1189,7 +1192,7 @@
       <c r="H5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="13"/>
       <c r="K5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1606,21 +1609,21 @@
       </c>
     </row>
     <row r="17" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="12" t="s">
         <v>0</v>
       </c>
       <c r="K17" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F18" s="11"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="7" t="s">
         <v>13</v>
       </c>
@@ -1834,7 +1837,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{5061348E-7F02-4662-9A06-A4A1FDDB0217}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{BFE24FF7-7917-4E5E-AAD4-ADEEA6AAD807}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1845,8 +1848,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Step 1 vs Step 2'!K5:K5</xm:f>
-              <xm:sqref>K5</xm:sqref>
+              <xm:f>'Step 1 vs Step 2'!H18:H18</xm:f>
+              <xm:sqref>H18</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1866,7 +1869,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{BFE24FF7-7917-4E5E-AAD4-ADEEA6AAD807}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{5061348E-7F02-4662-9A06-A4A1FDDB0217}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1877,8 +1880,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Step 1 vs Step 2'!H18:H18</xm:f>
-              <xm:sqref>H18</xm:sqref>
+              <xm:f>'Step 1 vs Step 2'!K5:K5</xm:f>
+              <xm:sqref>K5</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1893,7 +1896,7 @@
   <dimension ref="B4:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,12 +1907,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="8" t="s">
         <v>30</v>
       </c>
@@ -2051,6 +2054,7 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
@@ -2065,7 +2069,7 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Step 3'!C5:C5</xm:f>
+              <xm:f>'Step 4'!C5:C5</xm:f>
               <xm:sqref>C5</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>

</xml_diff>